<commit_message>
borramos un dato malo
</commit_message>
<xml_diff>
--- a/data/Planilla conteo directo .xlsx
+++ b/data/Planilla conteo directo .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/59011/Downloads/avistamiento_ballenas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D112F1A1-2733-A340-A460-D3337B9E4A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C902254F-CE3E-524D-A5E6-242F9E11F191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25600" yWindow="-8000" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$C$1:$C$182</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$C$1:$C$181</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="165">
   <si>
     <t>Tabla 1</t>
   </si>
@@ -686,9 +686,6 @@
   </si>
   <si>
     <t xml:space="preserve">Se observa ballena muy costera y muy activa realizando saltos. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ballena a unos 3 km de la costa, frente a piedra iglesia. </t>
   </si>
   <si>
     <t xml:space="preserve">Ballena muy costera frente a caleta Huiro </t>
@@ -2119,13 +2116,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F182"/>
+  <dimension ref="A1:F181"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B178" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D187" sqref="D187"/>
+      <selection pane="bottomRight" activeCell="D189" sqref="D189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2189,7 +2186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>44821</v>
       </c>
@@ -2209,7 +2206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>44822</v>
       </c>
@@ -2229,7 +2226,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>44824</v>
       </c>
@@ -2249,7 +2246,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>44831</v>
       </c>
@@ -2269,7 +2266,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
         <v>44831</v>
       </c>
@@ -2289,7 +2286,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>44833</v>
       </c>
@@ -2309,7 +2306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
         <v>44834</v>
       </c>
@@ -2349,7 +2346,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
         <v>44843</v>
       </c>
@@ -2409,7 +2406,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="7">
         <v>44889</v>
       </c>
@@ -2549,7 +2546,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="7">
         <v>44953</v>
       </c>
@@ -2647,7 +2644,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="7">
         <v>44973</v>
       </c>
@@ -2707,7 +2704,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="7">
         <v>44987</v>
       </c>
@@ -2847,7 +2844,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="7">
         <v>45016</v>
       </c>
@@ -2927,7 +2924,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="7">
         <v>45018</v>
       </c>
@@ -3307,7 +3304,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="7">
         <v>45038</v>
       </c>
@@ -3467,7 +3464,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="7">
         <v>45052</v>
       </c>
@@ -3967,7 +3964,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="7">
         <v>45178</v>
       </c>
@@ -3987,7 +3984,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="7">
         <v>45178</v>
       </c>
@@ -4305,7 +4302,7 @@
       </c>
       <c r="F109" s="11"/>
     </row>
-    <row r="110" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="7">
         <v>45219</v>
       </c>
@@ -4465,7 +4462,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="7">
         <v>45243</v>
       </c>
@@ -4505,7 +4502,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="7">
         <v>45244</v>
       </c>
@@ -4545,7 +4542,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="7">
         <v>45250</v>
       </c>
@@ -4725,7 +4722,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="7">
         <v>45277</v>
       </c>
@@ -5065,7 +5062,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="7">
         <v>45332</v>
       </c>
@@ -5325,7 +5322,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A161" s="7">
         <v>45382</v>
       </c>
@@ -5447,19 +5444,19 @@
     </row>
     <row r="167" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A167" s="7">
-        <v>45544</v>
+        <v>45396</v>
       </c>
       <c r="B167" s="8">
-        <v>45413.708333333336</v>
+        <v>45413.375</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D167" s="10">
         <v>1</v>
       </c>
       <c r="E167" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F167" s="9" t="s">
         <v>149</v>
@@ -5467,10 +5464,10 @@
     </row>
     <row r="168" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A168" s="7">
-        <v>45396</v>
+        <v>45398</v>
       </c>
       <c r="B168" s="8">
-        <v>45413.375</v>
+        <v>45413.75</v>
       </c>
       <c r="C168" s="9" t="s">
         <v>122</v>
@@ -5487,16 +5484,16 @@
     </row>
     <row r="169" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A169" s="7">
-        <v>45398</v>
+        <v>45400</v>
       </c>
       <c r="B169" s="8">
-        <v>45413.75</v>
+        <v>45413.333333333336</v>
       </c>
       <c r="C169" s="9" t="s">
         <v>122</v>
       </c>
       <c r="D169" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E169" s="10">
         <v>3</v>
@@ -5510,16 +5507,16 @@
         <v>45400</v>
       </c>
       <c r="B170" s="8">
-        <v>45413.333333333336</v>
+        <v>45413.677777777775</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D170" s="10">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E170" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F170" s="9" t="s">
         <v>152</v>
@@ -5527,59 +5524,59 @@
     </row>
     <row r="171" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A171" s="7">
-        <v>45400</v>
+        <v>45402</v>
       </c>
       <c r="B171" s="8">
-        <v>45413.677777777775</v>
+        <v>45413.625</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="D171" s="10">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E171" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F171" s="9" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A172" s="7">
-        <v>45402</v>
+        <v>45403</v>
       </c>
       <c r="B172" s="8">
-        <v>45413.625</v>
+        <v>45413.430555555555</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>122</v>
+        <v>25</v>
       </c>
       <c r="D172" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E172" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F172" s="9" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A173" s="7">
         <v>45403</v>
       </c>
       <c r="B173" s="8">
-        <v>45413.430555555555</v>
+        <v>45413.444444444445</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>25</v>
+        <v>122</v>
       </c>
       <c r="D173" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E173" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F173" s="9" t="s">
         <v>155</v>
@@ -5587,16 +5584,16 @@
     </row>
     <row r="174" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A174" s="7">
-        <v>45403</v>
+        <v>45405</v>
       </c>
       <c r="B174" s="8">
-        <v>45413.444444444445</v>
+        <v>45413.445833333331</v>
       </c>
       <c r="C174" s="9" t="s">
         <v>122</v>
       </c>
       <c r="D174" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E174" s="10">
         <v>1</v>
@@ -5607,99 +5604,99 @@
     </row>
     <row r="175" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A175" s="7">
-        <v>45405</v>
+        <v>45409</v>
       </c>
       <c r="B175" s="8">
-        <v>45413.445833333331</v>
+        <v>45413.75</v>
       </c>
       <c r="C175" s="9" t="s">
         <v>122</v>
       </c>
       <c r="D175" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E175" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F175" s="9" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A176" s="7">
-        <v>45409</v>
+        <v>45413</v>
       </c>
       <c r="B176" s="8">
-        <v>45413.75</v>
+        <v>45415.75</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="D176" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E176" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F176" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A177" s="7">
-        <v>45413</v>
+        <v>45414</v>
       </c>
       <c r="B177" s="8">
-        <v>45415.75</v>
+        <v>45415.430555555555</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D177" s="10">
         <v>1</v>
       </c>
       <c r="E177" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F177" s="9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A178" s="7">
         <v>45414</v>
       </c>
       <c r="B178" s="8">
-        <v>45415.430555555555</v>
+        <v>45415.444444444445</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D178" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E178" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F178" s="9" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A179" s="7">
         <v>45414</v>
       </c>
       <c r="B179" s="8">
-        <v>45415.444444444445</v>
+        <v>45415.5</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="D179" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E179" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F179" s="9" t="s">
         <v>163</v>
@@ -5710,54 +5707,34 @@
         <v>45414</v>
       </c>
       <c r="B180" s="8">
-        <v>45415.5</v>
+        <v>45415.583333333336</v>
       </c>
       <c r="C180" s="9" t="s">
         <v>111</v>
       </c>
       <c r="D180" s="10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E180" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F180" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A181" s="7">
-        <v>45414</v>
-      </c>
-      <c r="B181" s="8">
-        <v>45415.583333333336</v>
-      </c>
-      <c r="C181" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D181" s="10">
-        <v>7</v>
-      </c>
-      <c r="E181" s="10">
-        <v>2</v>
-      </c>
-      <c r="F181" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A182" s="12"/>
-      <c r="B182" s="8"/>
-      <c r="C182" s="11"/>
-      <c r="D182" s="11"/>
-      <c r="E182" s="11"/>
-      <c r="F182" s="11"/>
+    <row r="181" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A181" s="12"/>
+      <c r="B181" s="8"/>
+      <c r="C181" s="11"/>
+      <c r="D181" s="11"/>
+      <c r="E181" s="11"/>
+      <c r="F181" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C182" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="C1:C181" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Lobo fino austral"/>
+        <filter val="Ballena azul  (Balaenoptera musculus)"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
fix ballena azul duplicado
</commit_message>
<xml_diff>
--- a/data/Planilla conteo directo .xlsx
+++ b/data/Planilla conteo directo .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/59011/Downloads/avistamiento_ballenas/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C902254F-CE3E-524D-A5E6-242F9E11F191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961072EE-CF39-2541-A2C6-8082549055AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25600" yWindow="-8000" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="164">
   <si>
     <t>Tabla 1</t>
   </si>
@@ -79,36 +79,6 @@
     <t xml:space="preserve">Se observaron desde la caleta Huiro, 2 ejemplares adultos navegando hacia el sur. Se observador junto a cientos de fardelas blancas y negras alimentandose. Estos individuos se encontraban muy carca de la costa a unos 700 metros de la costa aprox.    </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ballena azul  (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>Balaenoptera musculus</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>Se observo un ejemplar de ballena posiblemente azul. El ejemplar se encontraba a unos 4 kilomentros de la costa</t>
   </si>
   <si>
@@ -592,9 +562,6 @@
     <t xml:space="preserve">Ballena muy costera alimentándose </t>
   </si>
   <si>
-    <t>Ballena azul  (Balaenoptera musculus)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Se observa ballena azul, a unos 3 km de la costa. </t>
   </si>
   <si>
@@ -734,6 +701,9 @@
   </si>
   <si>
     <t>Se observo un grupo navegando hacia el sur</t>
+  </si>
+  <si>
+    <t>Ballena azul (Balaenoptera musculus)</t>
   </si>
 </sst>
 </file>
@@ -2119,10 +2089,10 @@
   <dimension ref="A1:F181"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D189" sqref="D189"/>
+      <selection pane="bottomRight" activeCell="I188" sqref="I187:I188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2186,7 +2156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>44821</v>
       </c>
@@ -2194,19 +2164,19 @@
         <v>1.708333333333333</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10">
+        <v>2</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="10">
-        <v>1</v>
-      </c>
-      <c r="E4" s="10">
-        <v>2</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>44822</v>
       </c>
@@ -2214,7 +2184,7 @@
         <v>1.458333333333333</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D5" s="10">
         <v>1</v>
@@ -2223,10 +2193,10 @@
         <v>2</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
         <v>44824</v>
       </c>
@@ -2234,7 +2204,7 @@
         <v>1.8125</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D6" s="10">
         <v>1</v>
@@ -2243,10 +2213,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>44831</v>
       </c>
@@ -2254,7 +2224,7 @@
         <v>1.458333333333333</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D7" s="10">
         <v>2</v>
@@ -2263,10 +2233,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
         <v>44831</v>
       </c>
@@ -2274,7 +2244,7 @@
         <v>1.75</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D8" s="10">
         <v>6</v>
@@ -2283,10 +2253,10 @@
         <v>2</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>44833</v>
       </c>
@@ -2294,7 +2264,7 @@
         <v>1.791666666666667</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D9" s="10">
         <v>3</v>
@@ -2303,10 +2273,10 @@
         <v>2</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
         <v>44834</v>
       </c>
@@ -2314,7 +2284,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D10" s="10">
         <v>4</v>
@@ -2323,7 +2293,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2334,7 +2304,7 @@
         <v>1.5625</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="10">
         <v>2</v>
@@ -2343,10 +2313,10 @@
         <v>3</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
         <v>44843</v>
       </c>
@@ -2354,7 +2324,7 @@
         <v>1.791666666666667</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D12" s="10">
         <v>2</v>
@@ -2363,7 +2333,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2374,7 +2344,7 @@
         <v>1.75</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="10">
         <v>2</v>
@@ -2383,7 +2353,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2394,7 +2364,7 @@
         <v>1.489583333333333</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="10">
         <v>1</v>
@@ -2403,10 +2373,10 @@
         <v>2</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="7">
         <v>44889</v>
       </c>
@@ -2414,7 +2384,7 @@
         <v>1.569444444444444</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D15" s="10">
         <v>2</v>
@@ -2423,7 +2393,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2434,7 +2404,7 @@
         <v>1.625</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="10">
         <v>2</v>
@@ -2443,7 +2413,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2454,7 +2424,7 @@
         <v>1.583333333333333</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="10">
         <v>1</v>
@@ -2463,7 +2433,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2474,7 +2444,7 @@
         <v>44933.5</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="10">
         <v>1</v>
@@ -2483,7 +2453,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2494,16 +2464,16 @@
         <v>44934.75</v>
       </c>
       <c r="C19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="10">
+        <v>4</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="D19" s="10">
-        <v>4</v>
-      </c>
-      <c r="E19" s="10">
-        <v>1</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2514,16 +2484,16 @@
         <v>44934.770833333336</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="10">
+        <v>1</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="D20" s="10">
-        <v>1</v>
-      </c>
-      <c r="E20" s="10">
-        <v>1</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2534,7 +2504,7 @@
         <v>44934.791666666664</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="10">
         <v>1</v>
@@ -2543,10 +2513,10 @@
         <v>1</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="7">
         <v>44953</v>
       </c>
@@ -2554,7 +2524,7 @@
         <v>44957.711111111108</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D22" s="10">
         <v>2</v>
@@ -2563,7 +2533,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2574,7 +2544,7 @@
         <v>44957.791666666664</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="10">
         <v>2</v>
@@ -2583,7 +2553,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2594,7 +2564,7 @@
         <v>44990.479166666664</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="10">
         <v>3</v>
@@ -2603,7 +2573,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2614,7 +2584,7 @@
         <v>44990.75</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="10">
         <v>2</v>
@@ -2632,7 +2602,7 @@
         <v>44990.666666666664</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="10">
         <v>4</v>
@@ -2641,10 +2611,10 @@
         <v>2</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="7">
         <v>44973</v>
       </c>
@@ -2652,7 +2622,7 @@
         <v>44990.520833333336</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D27" s="10">
         <v>1</v>
@@ -2661,7 +2631,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2672,7 +2642,7 @@
         <v>44990.770833333336</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28" s="10">
         <v>1</v>
@@ -2681,7 +2651,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2692,7 +2662,7 @@
         <v>44990.645833333336</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="10">
         <v>1</v>
@@ -2701,10 +2671,10 @@
         <v>2</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="7">
         <v>44987</v>
       </c>
@@ -2712,7 +2682,7 @@
         <v>44994.688888888886</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D30" s="10">
         <v>1</v>
@@ -2721,7 +2691,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2732,7 +2702,7 @@
         <v>45008.666666666664</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="10">
         <v>2</v>
@@ -2741,7 +2711,7 @@
         <v>4</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2752,7 +2722,7 @@
         <v>45016.541666666664</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D32" s="10">
         <v>2</v>
@@ -2761,7 +2731,7 @@
         <v>4</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2772,7 +2742,7 @@
         <v>45016.458333333336</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="10">
         <v>1</v>
@@ -2781,7 +2751,7 @@
         <v>4</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2792,7 +2762,7 @@
         <v>45016.5</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D34" s="10">
         <v>1</v>
@@ -2801,7 +2771,7 @@
         <v>4</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2812,7 +2782,7 @@
         <v>45016.75</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35" s="10">
         <v>1</v>
@@ -2821,7 +2791,7 @@
         <v>2</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2832,7 +2802,7 @@
         <v>45016.583333333336</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D36" s="10">
         <v>2</v>
@@ -2841,10 +2811,10 @@
         <v>4</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="7">
         <v>45016</v>
       </c>
@@ -2852,7 +2822,7 @@
         <v>45016.583333333336</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D37" s="10">
         <v>1</v>
@@ -2861,7 +2831,7 @@
         <v>2</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2872,16 +2842,16 @@
         <v>45016.75</v>
       </c>
       <c r="C38" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1</v>
+      </c>
+      <c r="E38" s="10">
+        <v>2</v>
+      </c>
+      <c r="F38" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="D38" s="10">
-        <v>1</v>
-      </c>
-      <c r="E38" s="10">
-        <v>2</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2892,7 +2862,7 @@
         <v>45019.75</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" s="10">
         <v>2</v>
@@ -2901,7 +2871,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2912,7 +2882,7 @@
         <v>45019.729166666664</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D40" s="10">
         <v>1</v>
@@ -2921,10 +2891,10 @@
         <v>3</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="7">
         <v>45018</v>
       </c>
@@ -2932,7 +2902,7 @@
         <v>45019.75</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D41" s="10">
         <v>4</v>
@@ -2941,7 +2911,7 @@
         <v>4</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2952,7 +2922,7 @@
         <v>45019.756944444445</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D42" s="10">
         <v>2</v>
@@ -2961,7 +2931,7 @@
         <v>4</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2972,7 +2942,7 @@
         <v>45019.760416666664</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D43" s="10">
         <v>1</v>
@@ -2981,7 +2951,7 @@
         <v>4</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -2992,7 +2962,7 @@
         <v>45020.583333333336</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D44" s="10">
         <v>2</v>
@@ -3001,7 +2971,7 @@
         <v>4</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3012,7 +2982,7 @@
         <v>45020.5</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" s="10">
         <v>2</v>
@@ -3021,7 +2991,7 @@
         <v>4</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3032,7 +3002,7 @@
         <v>45030.645833333336</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D46" s="10">
         <v>2</v>
@@ -3041,7 +3011,7 @@
         <v>4</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3052,7 +3022,7 @@
         <v>45030.375</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D47" s="10">
         <v>2</v>
@@ -3061,7 +3031,7 @@
         <v>3</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3072,7 +3042,7 @@
         <v>45030.333333333336</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D48" s="10">
         <v>2</v>
@@ -3081,7 +3051,7 @@
         <v>2</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3092,7 +3062,7 @@
         <v>45030.75</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D49" s="10">
         <v>2</v>
@@ -3101,7 +3071,7 @@
         <v>4</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3112,7 +3082,7 @@
         <v>45042.5625</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D50" s="10">
         <v>2</v>
@@ -3121,7 +3091,7 @@
         <v>2</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3132,7 +3102,7 @@
         <v>45042.375</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D51" s="10">
         <v>2</v>
@@ -3141,7 +3111,7 @@
         <v>3</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3152,7 +3122,7 @@
         <v>45042.322916666664</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D52" s="10">
         <v>2</v>
@@ -3161,7 +3131,7 @@
         <v>3</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3172,7 +3142,7 @@
         <v>45042.666666666664</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D53" s="10">
         <v>1</v>
@@ -3181,7 +3151,7 @@
         <v>4</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3192,7 +3162,7 @@
         <v>45042.67291666667</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D54" s="10">
         <v>2</v>
@@ -3201,7 +3171,7 @@
         <v>2</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3212,7 +3182,7 @@
         <v>45042.4375</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D55" s="10">
         <v>2</v>
@@ -3221,7 +3191,7 @@
         <v>4</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3232,7 +3202,7 @@
         <v>45042.555555555555</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D56" s="10">
         <v>1</v>
@@ -3241,7 +3211,7 @@
         <v>2</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3252,7 +3222,7 @@
         <v>45042.541666666664</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D57" s="10">
         <v>2</v>
@@ -3261,7 +3231,7 @@
         <v>3</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3272,7 +3242,7 @@
         <v>45042.6875</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D58" s="10">
         <v>2</v>
@@ -3281,7 +3251,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3292,7 +3262,7 @@
         <v>45042.520833333336</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D59" s="10">
         <v>2</v>
@@ -3301,10 +3271,10 @@
         <v>2</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="7">
         <v>45038</v>
       </c>
@@ -3312,7 +3282,7 @@
         <v>45042.583333333336</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D60" s="10">
         <v>1</v>
@@ -3321,7 +3291,7 @@
         <v>1</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3332,7 +3302,7 @@
         <v>45042.583333333336</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D61" s="10">
         <v>2</v>
@@ -3341,7 +3311,7 @@
         <v>2</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3352,7 +3322,7 @@
         <v>45042.479166666664</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D62" s="10">
         <v>2</v>
@@ -3361,7 +3331,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3372,7 +3342,7 @@
         <v>45042.489583333336</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D63" s="10">
         <v>2</v>
@@ -3381,7 +3351,7 @@
         <v>2</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3392,7 +3362,7 @@
         <v>45042.443749999999</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D64" s="10">
         <v>2</v>
@@ -3401,7 +3371,7 @@
         <v>2</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3412,7 +3382,7 @@
         <v>45042.666666666664</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D65" s="10">
         <v>1</v>
@@ -3421,7 +3391,7 @@
         <v>1</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3432,7 +3402,7 @@
         <v>45042.416666666664</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D66" s="10">
         <v>2</v>
@@ -3441,7 +3411,7 @@
         <v>2</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3452,7 +3422,7 @@
         <v>45059.666666666664</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D67" s="10">
         <v>2</v>
@@ -3461,10 +3431,10 @@
         <v>2</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="7">
         <v>45052</v>
       </c>
@@ -3472,7 +3442,7 @@
         <v>45059.4375</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D68" s="10">
         <v>1</v>
@@ -3481,7 +3451,7 @@
         <v>2</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3492,7 +3462,7 @@
         <v>45096.458333333336</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D69" s="10">
         <v>30</v>
@@ -3501,7 +3471,7 @@
         <v>4</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3512,7 +3482,7 @@
         <v>45096.5625</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D70" s="10">
         <v>42</v>
@@ -3521,7 +3491,7 @@
         <v>4</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3532,7 +3502,7 @@
         <v>45096.583333333336</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D71" s="10">
         <v>50</v>
@@ -3541,7 +3511,7 @@
         <v>4</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3552,7 +3522,7 @@
         <v>45096.604166666664</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D72" s="10">
         <v>50</v>
@@ -3561,7 +3531,7 @@
         <v>4</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3572,7 +3542,7 @@
         <v>45142.458333333336</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D73" s="10">
         <v>20</v>
@@ -3581,7 +3551,7 @@
         <v>4</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3592,7 +3562,7 @@
         <v>45142.666666666664</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D74" s="10">
         <v>35</v>
@@ -3601,7 +3571,7 @@
         <v>4</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3612,7 +3582,7 @@
         <v>45142.416666666664</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D75" s="10">
         <v>25</v>
@@ -3621,7 +3591,7 @@
         <v>4</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3632,7 +3602,7 @@
         <v>45142.375</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D76" s="10">
         <v>40</v>
@@ -3641,7 +3611,7 @@
         <v>4</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3652,7 +3622,7 @@
         <v>45142.5</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D77" s="10">
         <v>32</v>
@@ -3661,7 +3631,7 @@
         <v>4</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3672,7 +3642,7 @@
         <v>45142.604166666664</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D78" s="10">
         <v>50</v>
@@ -3681,7 +3651,7 @@
         <v>4</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3692,7 +3662,7 @@
         <v>45142.729166666664</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D79" s="10">
         <v>50</v>
@@ -3701,7 +3671,7 @@
         <v>4</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3712,7 +3682,7 @@
         <v>45142.416666666664</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D80" s="10">
         <v>25</v>
@@ -3721,7 +3691,7 @@
         <v>4</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3732,7 +3702,7 @@
         <v>45142.729166666664</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D81" s="10">
         <v>30</v>
@@ -3741,7 +3711,7 @@
         <v>4</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3752,7 +3722,7 @@
         <v>45142.513888888891</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D82" s="10">
         <v>40</v>
@@ -3761,7 +3731,7 @@
         <v>4</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3772,7 +3742,7 @@
         <v>45142.416666666664</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D83" s="10">
         <v>25</v>
@@ -3781,7 +3751,7 @@
         <v>4</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3792,7 +3762,7 @@
         <v>45142.583333333336</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D84" s="10">
         <v>20</v>
@@ -3801,7 +3771,7 @@
         <v>4</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3812,7 +3782,7 @@
         <v>45142.583333333336</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D85" s="10">
         <v>1</v>
@@ -3821,7 +3791,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3832,7 +3802,7 @@
         <v>45142.708333333336</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D86" s="10">
         <v>4</v>
@@ -3841,7 +3811,7 @@
         <v>3</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3852,7 +3822,7 @@
         <v>45142.416666666664</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D87" s="10">
         <v>30</v>
@@ -3861,7 +3831,7 @@
         <v>4</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3872,7 +3842,7 @@
         <v>45142.583333333336</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D88" s="10">
         <v>25</v>
@@ -3881,7 +3851,7 @@
         <v>4</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3892,7 +3862,7 @@
         <v>45180.666666666664</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D89" s="10">
         <v>6</v>
@@ -3901,7 +3871,7 @@
         <v>4</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3912,7 +3882,7 @@
         <v>45180.458333333336</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D90" s="10">
         <v>25</v>
@@ -3921,7 +3891,7 @@
         <v>4</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3932,7 +3902,7 @@
         <v>45180.708333333336</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D91" s="10">
         <v>10</v>
@@ -3941,7 +3911,7 @@
         <v>4</v>
       </c>
       <c r="F91" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3952,7 +3922,7 @@
         <v>45180.645833333336</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D92" s="10">
         <v>12</v>
@@ -3961,10 +3931,10 @@
         <v>1</v>
       </c>
       <c r="F92" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="7">
         <v>45178</v>
       </c>
@@ -3972,7 +3942,7 @@
         <v>45180.666666666664</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D93" s="10">
         <v>3</v>
@@ -3981,10 +3951,10 @@
         <v>1</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="7">
         <v>45178</v>
       </c>
@@ -3992,7 +3962,7 @@
         <v>45180.6875</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D94" s="10">
         <v>1</v>
@@ -4001,7 +3971,7 @@
         <v>2</v>
       </c>
       <c r="F94" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4012,7 +3982,7 @@
         <v>45192.770833333336</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D95" s="10">
         <v>3</v>
@@ -4021,7 +3991,7 @@
         <v>4</v>
       </c>
       <c r="F95" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4032,7 +4002,7 @@
         <v>45192.765972222223</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D96" s="10">
         <v>2</v>
@@ -4041,7 +4011,7 @@
         <v>2</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4061,7 +4031,7 @@
         <v>2</v>
       </c>
       <c r="F97" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4072,7 +4042,7 @@
         <v>45236.416666666664</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D98" s="10">
         <v>1</v>
@@ -4081,7 +4051,7 @@
         <v>2</v>
       </c>
       <c r="F98" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4092,7 +4062,7 @@
         <v>45236.493055555555</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D99" s="10">
         <v>15</v>
@@ -4101,7 +4071,7 @@
         <v>4</v>
       </c>
       <c r="F99" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4112,7 +4082,7 @@
         <v>45236.458333333336</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D100" s="10">
         <v>1</v>
@@ -4121,7 +4091,7 @@
         <v>3</v>
       </c>
       <c r="F100" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4132,7 +4102,7 @@
         <v>45236.790277777778</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D101" s="10">
         <v>1</v>
@@ -4141,7 +4111,7 @@
         <v>3</v>
       </c>
       <c r="F101" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4152,7 +4122,7 @@
         <v>45236.449305555558</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D102" s="10">
         <v>1</v>
@@ -4161,7 +4131,7 @@
         <v>2</v>
       </c>
       <c r="F102" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4172,7 +4142,7 @@
         <v>45236.638888888891</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D103" s="10">
         <v>1</v>
@@ -4181,7 +4151,7 @@
         <v>2</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4192,7 +4162,7 @@
         <v>45236.493055555555</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D104" s="10">
         <v>5</v>
@@ -4201,7 +4171,7 @@
         <v>2</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4212,7 +4182,7 @@
         <v>45236.566666666666</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D105" s="10">
         <v>1</v>
@@ -4221,7 +4191,7 @@
         <v>1</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4232,7 +4202,7 @@
         <v>45236.479166666664</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D106" s="10">
         <v>3</v>
@@ -4241,7 +4211,7 @@
         <v>3</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4252,7 +4222,7 @@
         <v>45236.48333333333</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D107" s="10">
         <v>1</v>
@@ -4261,7 +4231,7 @@
         <v>3</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4272,7 +4242,7 @@
         <v>45236.708333333336</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D108" s="10">
         <v>1</v>
@@ -4281,7 +4251,7 @@
         <v>2</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4292,7 +4262,7 @@
         <v>45236.450694444444</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D109" s="10">
         <v>1</v>
@@ -4302,7 +4272,7 @@
       </c>
       <c r="F109" s="11"/>
     </row>
-    <row r="110" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="7">
         <v>45219</v>
       </c>
@@ -4310,7 +4280,7 @@
         <v>45236.477083333331</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D110" s="10">
         <v>1</v>
@@ -4319,7 +4289,7 @@
         <v>1</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4330,7 +4300,7 @@
         <v>45236.549305555556</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D111" s="10">
         <v>5</v>
@@ -4339,7 +4309,7 @@
         <v>2</v>
       </c>
       <c r="F111" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4350,7 +4320,7 @@
         <v>45236.68472222222</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D112" s="10">
         <v>1</v>
@@ -4359,7 +4329,7 @@
         <v>2</v>
       </c>
       <c r="F112" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4370,7 +4340,7 @@
         <v>45236.690972222219</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D113" s="10">
         <v>1</v>
@@ -4379,7 +4349,7 @@
         <v>4</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4390,7 +4360,7 @@
         <v>45236.513888888891</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D114" s="10">
         <v>6</v>
@@ -4399,7 +4369,7 @@
         <v>2</v>
       </c>
       <c r="F114" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4410,7 +4380,7 @@
         <v>45236.5</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D115" s="10">
         <v>12</v>
@@ -4419,7 +4389,7 @@
         <v>3</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4430,7 +4400,7 @@
         <v>45236.625</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D116" s="10">
         <v>8</v>
@@ -4439,7 +4409,7 @@
         <v>3</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4450,7 +4420,7 @@
         <v>45236.527777777781</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D117" s="10">
         <v>6</v>
@@ -4459,10 +4429,10 @@
         <v>3</v>
       </c>
       <c r="F117" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="7">
         <v>45243</v>
       </c>
@@ -4470,7 +4440,7 @@
         <v>45266.791666666664</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D118" s="10">
         <v>3</v>
@@ -4479,7 +4449,7 @@
         <v>2</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4490,7 +4460,7 @@
         <v>45266.8125</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D119" s="10">
         <v>2</v>
@@ -4499,10 +4469,10 @@
         <v>2</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="7">
         <v>45244</v>
       </c>
@@ -4510,7 +4480,7 @@
         <v>45266.824305555558</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D120" s="10">
         <v>1</v>
@@ -4519,7 +4489,7 @@
         <v>2</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4530,7 +4500,7 @@
         <v>45266.708333333336</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D121" s="10">
         <v>2</v>
@@ -4539,10 +4509,10 @@
         <v>2</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="7">
         <v>45250</v>
       </c>
@@ -4550,7 +4520,7 @@
         <v>45266.645833333336</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="D122" s="10">
         <v>1</v>
@@ -4559,7 +4529,7 @@
         <v>2</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4579,7 +4549,7 @@
         <v>4</v>
       </c>
       <c r="F123" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4590,7 +4560,7 @@
         <v>45266.458333333336</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D124" s="10">
         <v>7</v>
@@ -4599,7 +4569,7 @@
         <v>4</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4610,7 +4580,7 @@
         <v>45266.5625</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D125" s="10">
         <v>3</v>
@@ -4619,7 +4589,7 @@
         <v>4</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4630,16 +4600,16 @@
         <v>45373.397916666669</v>
       </c>
       <c r="C126" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D126" s="10">
+        <v>2</v>
+      </c>
+      <c r="E126" s="10">
+        <v>2</v>
+      </c>
+      <c r="F126" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="D126" s="10">
-        <v>2</v>
-      </c>
-      <c r="E126" s="10">
-        <v>2</v>
-      </c>
-      <c r="F126" s="9" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4650,7 +4620,7 @@
         <v>45373.426388888889</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D127" s="10">
         <v>10</v>
@@ -4659,7 +4629,7 @@
         <v>2</v>
       </c>
       <c r="F127" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4670,7 +4640,7 @@
         <v>45373.839583333334</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D128" s="10">
         <v>1</v>
@@ -4679,7 +4649,7 @@
         <v>3</v>
       </c>
       <c r="F128" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4690,7 +4660,7 @@
         <v>45373.468055555553</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D129" s="10">
         <v>6</v>
@@ -4699,7 +4669,7 @@
         <v>1</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4710,7 +4680,7 @@
         <v>45373.633333333331</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D130" s="10">
         <v>1</v>
@@ -4719,10 +4689,10 @@
         <v>2</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="7">
         <v>45277</v>
       </c>
@@ -4730,7 +4700,7 @@
         <v>45373.634722222225</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>117</v>
+        <v>163</v>
       </c>
       <c r="D131" s="10">
         <v>1</v>
@@ -4739,7 +4709,7 @@
         <v>2</v>
       </c>
       <c r="F131" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4750,7 +4720,7 @@
         <v>45373.691666666666</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D132" s="10">
         <v>1</v>
@@ -4759,7 +4729,7 @@
         <v>2</v>
       </c>
       <c r="F132" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4770,7 +4740,7 @@
         <v>45373.45416666667</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D133" s="10">
         <v>12</v>
@@ -4779,7 +4749,7 @@
         <v>4</v>
       </c>
       <c r="F133" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4790,7 +4760,7 @@
         <v>45373.588888888888</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D134" s="10">
         <v>1</v>
@@ -4799,7 +4769,7 @@
         <v>3</v>
       </c>
       <c r="F134" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4810,7 +4780,7 @@
         <v>45373.680555555555</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D135" s="10">
         <v>1</v>
@@ -4819,7 +4789,7 @@
         <v>2</v>
       </c>
       <c r="F135" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4830,7 +4800,7 @@
         <v>45373.854166666664</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D136" s="10">
         <v>12</v>
@@ -4839,7 +4809,7 @@
         <v>4</v>
       </c>
       <c r="F136" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4850,7 +4820,7 @@
         <v>45373.857638888891</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D137" s="10">
         <v>2</v>
@@ -4859,7 +4829,7 @@
         <v>4</v>
       </c>
       <c r="F137" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4870,7 +4840,7 @@
         <v>45373.842361111114</v>
       </c>
       <c r="C138" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D138" s="10">
         <v>3</v>
@@ -4879,7 +4849,7 @@
         <v>4</v>
       </c>
       <c r="F138" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4890,7 +4860,7 @@
         <v>45373.727777777778</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D139" s="10">
         <v>5</v>
@@ -4899,7 +4869,7 @@
         <v>4</v>
       </c>
       <c r="F139" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="140" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4910,7 +4880,7 @@
         <v>45373.822916666664</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D140" s="10">
         <v>1</v>
@@ -4919,7 +4889,7 @@
         <v>4</v>
       </c>
       <c r="F140" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4930,7 +4900,7 @@
         <v>45373.538194444445</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D141" s="10">
         <v>10</v>
@@ -4939,7 +4909,7 @@
         <v>3</v>
       </c>
       <c r="F141" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="142" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4950,7 +4920,7 @@
         <v>45373.7</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D142" s="10">
         <v>1</v>
@@ -4959,7 +4929,7 @@
         <v>2</v>
       </c>
       <c r="F142" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4970,7 +4940,7 @@
         <v>45373.785416666666</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D143" s="10">
         <v>2</v>
@@ -4979,7 +4949,7 @@
         <v>4</v>
       </c>
       <c r="F143" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -4990,7 +4960,7 @@
         <v>45373.5</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D144" s="10">
         <v>2</v>
@@ -4999,7 +4969,7 @@
         <v>4</v>
       </c>
       <c r="F144" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5010,7 +4980,7 @@
         <v>45373.722916666666</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D145" s="10">
         <v>1</v>
@@ -5019,7 +4989,7 @@
         <v>3</v>
       </c>
       <c r="F145" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5030,7 +5000,7 @@
         <v>45373.723611111112</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D146" s="10">
         <v>3</v>
@@ -5039,7 +5009,7 @@
         <v>2</v>
       </c>
       <c r="F146" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5050,7 +5020,7 @@
         <v>45373.729166666664</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D147" s="10">
         <v>2</v>
@@ -5059,10 +5029,10 @@
         <v>3</v>
       </c>
       <c r="F147" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="7">
         <v>45332</v>
       </c>
@@ -5070,7 +5040,7 @@
         <v>45373.813194444447</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>117</v>
+        <v>163</v>
       </c>
       <c r="D148" s="10">
         <v>1</v>
@@ -5079,7 +5049,7 @@
         <v>2</v>
       </c>
       <c r="F148" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5090,7 +5060,7 @@
         <v>45373.68472222222</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D149" s="10">
         <v>12</v>
@@ -5099,7 +5069,7 @@
         <v>4</v>
       </c>
       <c r="F149" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5110,7 +5080,7 @@
         <v>45373.479166666664</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D150" s="10">
         <v>6</v>
@@ -5119,7 +5089,7 @@
         <v>4</v>
       </c>
       <c r="F150" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5130,7 +5100,7 @@
         <v>45373.708333333336</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D151" s="10">
         <v>10</v>
@@ -5139,7 +5109,7 @@
         <v>4</v>
       </c>
       <c r="F151" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="152" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5150,7 +5120,7 @@
         <v>45373.436111111114</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D152" s="10">
         <v>7</v>
@@ -5159,7 +5129,7 @@
         <v>4</v>
       </c>
       <c r="F152" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="153" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5170,7 +5140,7 @@
         <v>45373.597222222219</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D153" s="10">
         <v>6</v>
@@ -5179,7 +5149,7 @@
         <v>4</v>
       </c>
       <c r="F153" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="154" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5190,7 +5160,7 @@
         <v>45373.813888888886</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D154" s="10">
         <v>8</v>
@@ -5199,7 +5169,7 @@
         <v>4</v>
       </c>
       <c r="F154" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="155" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5210,7 +5180,7 @@
         <v>45373.523611111108</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D155" s="10">
         <v>12</v>
@@ -5219,7 +5189,7 @@
         <v>4</v>
       </c>
       <c r="F155" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="156" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5230,7 +5200,7 @@
         <v>45373.472222222219</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D156" s="10">
         <v>4</v>
@@ -5239,7 +5209,7 @@
         <v>4</v>
       </c>
       <c r="F156" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5250,7 +5220,7 @@
         <v>45373.597222222219</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D157" s="10">
         <v>7</v>
@@ -5259,7 +5229,7 @@
         <v>4</v>
       </c>
       <c r="F157" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5270,7 +5240,7 @@
         <v>45389.760416666664</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D158" s="10">
         <v>1</v>
@@ -5279,7 +5249,7 @@
         <v>1</v>
       </c>
       <c r="F158" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5290,7 +5260,7 @@
         <v>45389.520833333336</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D159" s="10">
         <v>1</v>
@@ -5299,7 +5269,7 @@
         <v>2</v>
       </c>
       <c r="F159" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5310,7 +5280,7 @@
         <v>45389.822916666664</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D160" s="10">
         <v>1</v>
@@ -5319,10 +5289,10 @@
         <v>3</v>
       </c>
       <c r="F160" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A161" s="7">
         <v>45382</v>
       </c>
@@ -5330,7 +5300,7 @@
         <v>45389.429166666669</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>117</v>
+        <v>163</v>
       </c>
       <c r="D161" s="10">
         <v>1</v>
@@ -5339,7 +5309,7 @@
         <v>2</v>
       </c>
       <c r="F161" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5350,7 +5320,7 @@
         <v>45389.848611111112</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D162" s="10">
         <v>7</v>
@@ -5359,7 +5329,7 @@
         <v>4</v>
       </c>
       <c r="F162" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5370,7 +5340,7 @@
         <v>45389.742361111108</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D163" s="10">
         <v>1</v>
@@ -5379,7 +5349,7 @@
         <v>2</v>
       </c>
       <c r="F163" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5390,7 +5360,7 @@
         <v>45389.667361111111</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D164" s="10">
         <v>1</v>
@@ -5399,7 +5369,7 @@
         <v>2</v>
       </c>
       <c r="F164" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5410,7 +5380,7 @@
         <v>45389.572222222225</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D165" s="10">
         <v>1</v>
@@ -5419,7 +5389,7 @@
         <v>2</v>
       </c>
       <c r="F165" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5430,7 +5400,7 @@
         <v>45413.625</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D166" s="10">
         <v>1</v>
@@ -5439,7 +5409,7 @@
         <v>4</v>
       </c>
       <c r="F166" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5450,7 +5420,7 @@
         <v>45413.375</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D167" s="10">
         <v>1</v>
@@ -5459,7 +5429,7 @@
         <v>3</v>
       </c>
       <c r="F167" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5470,7 +5440,7 @@
         <v>45413.75</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D168" s="10">
         <v>1</v>
@@ -5479,7 +5449,7 @@
         <v>3</v>
       </c>
       <c r="F168" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5490,7 +5460,7 @@
         <v>45413.333333333336</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D169" s="10">
         <v>2</v>
@@ -5499,7 +5469,7 @@
         <v>3</v>
       </c>
       <c r="F169" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5510,7 +5480,7 @@
         <v>45413.677777777775</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D170" s="10">
         <v>22</v>
@@ -5519,7 +5489,7 @@
         <v>4</v>
       </c>
       <c r="F170" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5530,7 +5500,7 @@
         <v>45413.625</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D171" s="10">
         <v>1</v>
@@ -5539,7 +5509,7 @@
         <v>3</v>
       </c>
       <c r="F171" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5550,7 +5520,7 @@
         <v>45413.430555555555</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D172" s="10">
         <v>5</v>
@@ -5559,7 +5529,7 @@
         <v>2</v>
       </c>
       <c r="F172" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5570,7 +5540,7 @@
         <v>45413.444444444445</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D173" s="10">
         <v>2</v>
@@ -5579,7 +5549,7 @@
         <v>1</v>
       </c>
       <c r="F173" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5590,7 +5560,7 @@
         <v>45413.445833333331</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D174" s="10">
         <v>1</v>
@@ -5599,7 +5569,7 @@
         <v>1</v>
       </c>
       <c r="F174" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5610,7 +5580,7 @@
         <v>45413.75</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D175" s="10">
         <v>2</v>
@@ -5619,7 +5589,7 @@
         <v>2</v>
       </c>
       <c r="F175" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5630,7 +5600,7 @@
         <v>45415.75</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D176" s="10">
         <v>1</v>
@@ -5639,7 +5609,7 @@
         <v>4</v>
       </c>
       <c r="F176" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5650,7 +5620,7 @@
         <v>45415.430555555555</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D177" s="10">
         <v>1</v>
@@ -5659,7 +5629,7 @@
         <v>3</v>
       </c>
       <c r="F177" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="32" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5670,16 +5640,16 @@
         <v>45415.444444444445</v>
       </c>
       <c r="C178" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D178" s="10">
+        <v>2</v>
+      </c>
+      <c r="E178" s="10">
+        <v>2</v>
+      </c>
+      <c r="F178" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="D178" s="10">
-        <v>2</v>
-      </c>
-      <c r="E178" s="10">
-        <v>2</v>
-      </c>
-      <c r="F178" s="9" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5690,7 +5660,7 @@
         <v>45415.5</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D179" s="10">
         <v>5</v>
@@ -5699,7 +5669,7 @@
         <v>4</v>
       </c>
       <c r="F179" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="44" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -5710,7 +5680,7 @@
         <v>45415.583333333336</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D180" s="10">
         <v>7</v>
@@ -5719,10 +5689,10 @@
         <v>2</v>
       </c>
       <c r="F180" s="9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A181" s="12"/>
       <c r="B181" s="8"/>
       <c r="C181" s="11"/>
@@ -5733,9 +5703,7 @@
   </sheetData>
   <autoFilter ref="C1:C181" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
-      <filters>
-        <filter val="Ballena azul  (Balaenoptera musculus)"/>
-      </filters>
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <mergeCells count="1">

</xml_diff>